<commit_message>
Se actualiza el script para subir el archivo Donaciones_2017.xlsx
</commit_message>
<xml_diff>
--- a/DonacionesProyectos.xlsx
+++ b/DonacionesProyectos.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matia\OneDrive\Documentos\GitHub\desafio1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06AEB8CC-41DD-4A6B-93EA-A07844978384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{94E1DA2B-1C89-4E7C-B98C-CEF422AF413C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
-    <sheet name="DonacionesProyectos" sheetId="1" r:id="rId1"/>
+    <sheet name="DonacionesProyectos (2)" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -5801,7 +5801,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO659"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>